<commit_message>
Change app state data to json.
</commit_message>
<xml_diff>
--- a/product_ids.xlsx
+++ b/product_ids.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olorin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\wildberries_parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C6E413B-FC26-4661-894C-875A442B6008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AB68AF-801C-452C-AA4B-28ECC9236E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1551277-44E3-489D-97BB-BFAF6A04487A}"/>
   </bookViews>
@@ -392,7 +392,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>